<commit_message>
fixed image invalid url bypass, fixed product model by adding 4 new fields (arabic/english retail unit, arabic/english wholesale unit). removed linux, windows, macos, web support due to deprecation.
</commit_message>
<xml_diff>
--- a/assets/Products sheet.xlsx
+++ b/assets/Products sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Programming Projects\Flutter Projects\magazine\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdbm\Projects\FlutterProjects\thraa_najd_app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553BA369-B73C-4DB2-A819-82E59E37DE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C24EAA7-E154-47D8-9D01-EF1E032BF8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{949728EA-1729-4725-BCDE-92DD77268081}"/>
+    <workbookView xWindow="3105" yWindow="2010" windowWidth="15375" windowHeight="7995" xr2:uid="{949728EA-1729-4725-BCDE-92DD77268081}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="296">
   <si>
     <t>01001</t>
   </si>
@@ -886,9 +886,6 @@
     <t>باكينغ بودر نوع اول  5 كغ</t>
   </si>
   <si>
-    <t>مكسرات</t>
-  </si>
-  <si>
     <t>productNameAR</t>
   </si>
   <si>
@@ -898,9 +895,6 @@
     <t>materialId</t>
   </si>
   <si>
-    <t>categoryAR</t>
-  </si>
-  <si>
     <t>categoryEN</t>
   </si>
   <si>
@@ -911,6 +905,24 @@
   </si>
   <si>
     <t>nuts</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>wholesaleUnutEN</t>
+  </si>
+  <si>
+    <t>retailUnitAR</t>
+  </si>
+  <si>
+    <t>سس</t>
+  </si>
+  <si>
+    <t>retailUnitEN</t>
+  </si>
+  <si>
+    <t>wholesaleUnitAR</t>
   </si>
 </sst>
 </file>
@@ -1424,48 +1436,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9675C5BC-2F81-441D-A9E9-EE0B24CBC063}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="38.375" customWidth="1"/>
     <col min="3" max="3" width="25.125" customWidth="1"/>
-    <col min="4" max="5" width="25.125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="11.25" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="11.25" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="12.375" customWidth="1"/>
     <col min="12" max="12" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>287</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8">
+        <v>292</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1476,20 +1499,25 @@
         <v>2</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="F2" s="7">
+        <v>289</v>
+      </c>
+      <c r="E2" s="7">
         <v>1080</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="G2" t="s">
+        <v>293</v>
+      </c>
+      <c r="H2" t="s">
+        <v>293</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>93</v>
       </c>
@@ -1500,16 +1528,17 @@
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="14">
+      <c r="E3" s="14">
         <v>550</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>94</v>
       </c>
@@ -1520,16 +1549,17 @@
         <v>4</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7">
+      <c r="E4" s="7">
         <v>103</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="F4" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>95</v>
       </c>
@@ -1540,16 +1570,17 @@
         <v>5</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="14">
+      <c r="E5" s="14">
         <v>240</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>96</v>
       </c>
@@ -1560,13 +1591,12 @@
         <v>6</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7">
+      <c r="E6" s="7">
         <v>1080</v>
       </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>97</v>
       </c>
@@ -1577,13 +1607,12 @@
         <v>7</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="14">
+      <c r="E7" s="14">
         <v>150</v>
       </c>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>98</v>
       </c>
@@ -1594,13 +1623,12 @@
         <v>8</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7">
+      <c r="E8" s="7">
         <v>550</v>
       </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>99</v>
       </c>
@@ -1611,13 +1639,12 @@
         <v>9</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="14">
+      <c r="E9" s="14">
         <v>108</v>
       </c>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>100</v>
       </c>
@@ -1628,13 +1655,12 @@
         <v>10</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7">
+      <c r="E10" s="7">
         <v>60</v>
       </c>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>101</v>
       </c>
@@ -1645,13 +1671,12 @@
         <v>11</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="14">
+      <c r="E11" s="14">
         <v>420</v>
       </c>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>102</v>
       </c>
@@ -1662,13 +1687,12 @@
         <v>12</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7">
+      <c r="E12" s="7">
         <v>230</v>
       </c>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
         <v>103</v>
       </c>
@@ -1679,13 +1703,12 @@
         <v>13</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="14">
+      <c r="E13" s="14">
         <v>230</v>
       </c>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
         <v>104</v>
       </c>
@@ -1696,13 +1719,12 @@
         <v>14</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7">
+      <c r="E14" s="7">
         <v>100</v>
       </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="17" t="s">
         <v>105</v>
       </c>
@@ -1713,13 +1735,12 @@
         <v>15</v>
       </c>
       <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="20">
+      <c r="E15" s="20">
         <v>195</v>
       </c>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>106</v>
       </c>
@@ -1730,13 +1751,12 @@
         <v>16</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7">
+      <c r="E16" s="7">
         <v>16.72</v>
       </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
         <v>107</v>
       </c>
@@ -1747,13 +1767,12 @@
         <v>17</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="14">
+      <c r="E17" s="14">
         <v>230</v>
       </c>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>108</v>
       </c>
@@ -1764,13 +1783,12 @@
         <v>18</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7">
+      <c r="E18" s="7">
         <v>255</v>
       </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>109</v>
       </c>
@@ -1781,13 +1799,12 @@
         <v>19</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="14">
+      <c r="E19" s="14">
         <v>110</v>
       </c>
-      <c r="H19" s="14"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>110</v>
       </c>
@@ -1798,13 +1815,12 @@
         <v>20</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7">
+      <c r="E20" s="7">
         <v>235</v>
       </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>111</v>
       </c>
@@ -1815,13 +1831,12 @@
         <v>21</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="14">
+      <c r="E21" s="14">
         <v>87</v>
       </c>
-      <c r="H21" s="14"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
         <v>112</v>
       </c>
@@ -1832,13 +1847,12 @@
         <v>22</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7">
+      <c r="E22" s="7">
         <v>950</v>
       </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
         <v>113</v>
       </c>
@@ -1849,13 +1863,12 @@
         <v>23</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="14">
+      <c r="E23" s="14">
         <v>480</v>
       </c>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
         <v>114</v>
       </c>
@@ -1866,13 +1879,12 @@
         <v>24</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7">
+      <c r="E24" s="7">
         <v>360</v>
       </c>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
         <v>115</v>
       </c>
@@ -1883,13 +1895,12 @@
         <v>25</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="14">
+      <c r="E25" s="14">
         <v>18.399999999999999</v>
       </c>
-      <c r="H25" s="14"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
         <v>116</v>
       </c>
@@ -1900,13 +1911,12 @@
         <v>26</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7">
+      <c r="E26" s="7">
         <v>12</v>
       </c>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
         <v>117</v>
       </c>
@@ -1917,13 +1927,12 @@
         <v>27</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="14">
+      <c r="E27" s="14">
         <v>16</v>
       </c>
-      <c r="H27" s="14"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
         <v>118</v>
       </c>
@@ -1934,13 +1943,12 @@
         <v>28</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7">
+      <c r="E28" s="7">
         <v>20</v>
       </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="3" t="s">
         <v>119</v>
       </c>
@@ -1951,13 +1959,12 @@
         <v>29</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="14">
+      <c r="E29" s="14">
         <v>83</v>
       </c>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="G29" s="14"/>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
         <v>120</v>
       </c>
@@ -1968,13 +1975,12 @@
         <v>30</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7">
+      <c r="E30" s="7">
         <v>18</v>
       </c>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
         <v>121</v>
       </c>
@@ -1985,13 +1991,12 @@
         <v>31</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="14">
+      <c r="E31" s="14">
         <v>65</v>
       </c>
-      <c r="H31" s="14"/>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
         <v>122</v>
       </c>
@@ -2002,13 +2007,12 @@
         <v>32</v>
       </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7">
+      <c r="E32" s="7">
         <v>44</v>
       </c>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
         <v>123</v>
       </c>
@@ -2019,13 +2023,12 @@
         <v>33</v>
       </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="14">
+      <c r="E33" s="14">
         <v>50</v>
       </c>
-      <c r="H33" s="14"/>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
         <v>124</v>
       </c>
@@ -2036,13 +2039,12 @@
         <v>34</v>
       </c>
       <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7">
+      <c r="E34" s="7">
         <v>195</v>
       </c>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="3" t="s">
         <v>125</v>
       </c>
@@ -2053,13 +2055,12 @@
         <v>35</v>
       </c>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="14">
+      <c r="E35" s="14">
         <v>85</v>
       </c>
-      <c r="H35" s="14"/>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="3" t="s">
         <v>126</v>
       </c>
@@ -2070,13 +2071,12 @@
         <v>36</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7">
+      <c r="E36" s="7">
         <v>54</v>
       </c>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="3" t="s">
         <v>127</v>
       </c>
@@ -2087,13 +2087,12 @@
         <v>37</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="14">
+      <c r="E37" s="14">
         <v>95</v>
       </c>
-      <c r="H37" s="14"/>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="3" t="s">
         <v>128</v>
       </c>
@@ -2104,13 +2103,12 @@
         <v>38</v>
       </c>
       <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7">
+      <c r="E38" s="7">
         <v>59</v>
       </c>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="3" t="s">
         <v>129</v>
       </c>
@@ -2121,13 +2119,12 @@
         <v>39</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="14">
+      <c r="E39" s="14">
         <v>185</v>
       </c>
-      <c r="H39" s="14"/>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="3" t="s">
         <v>130</v>
       </c>
@@ -2138,13 +2135,12 @@
         <v>40</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7">
+      <c r="E40" s="7">
         <v>65</v>
       </c>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="3" t="s">
         <v>131</v>
       </c>
@@ -2155,13 +2151,12 @@
         <v>41</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="14">
+      <c r="E41" s="14">
         <v>26</v>
       </c>
-      <c r="H41" s="14"/>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="3" t="s">
         <v>132</v>
       </c>
@@ -2172,13 +2167,12 @@
         <v>42</v>
       </c>
       <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="7">
+      <c r="E42" s="7">
         <v>180</v>
       </c>
-      <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="3" t="s">
         <v>133</v>
       </c>
@@ -2189,13 +2183,12 @@
         <v>43</v>
       </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="14">
+      <c r="E43" s="14">
         <v>9</v>
       </c>
-      <c r="H43" s="14"/>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="3" t="s">
         <v>134</v>
       </c>
@@ -2206,13 +2199,12 @@
         <v>44</v>
       </c>
       <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="7">
+      <c r="E44" s="7">
         <v>3.5</v>
       </c>
-      <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="3" t="s">
         <v>135</v>
       </c>
@@ -2223,13 +2215,12 @@
         <v>45</v>
       </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="14">
+      <c r="E45" s="14">
         <v>87.5</v>
       </c>
-      <c r="H45" s="14"/>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="3" t="s">
         <v>136</v>
       </c>
@@ -2240,13 +2231,12 @@
         <v>46</v>
       </c>
       <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="7">
+      <c r="E46" s="7">
         <v>9</v>
       </c>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="3" t="s">
         <v>137</v>
       </c>
@@ -2257,13 +2247,12 @@
         <v>47</v>
       </c>
       <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="14">
+      <c r="E47" s="14">
         <v>90</v>
       </c>
-      <c r="H47" s="14"/>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="G47" s="14"/>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="3" t="s">
         <v>138</v>
       </c>
@@ -2274,13 +2263,12 @@
         <v>48</v>
       </c>
       <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="7">
+      <c r="E48" s="7">
         <v>9</v>
       </c>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="3" t="s">
         <v>139</v>
       </c>
@@ -2291,13 +2279,12 @@
         <v>49</v>
       </c>
       <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="14">
+      <c r="E49" s="14">
         <v>125</v>
       </c>
-      <c r="H49" s="14"/>
-    </row>
-    <row r="50" spans="1:8" s="25" customFormat="1">
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:7" s="25" customFormat="1">
       <c r="A50" s="21" t="s">
         <v>140</v>
       </c>
@@ -2308,13 +2295,12 @@
         <v>50</v>
       </c>
       <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="24">
+      <c r="E50" s="24">
         <v>126.09</v>
       </c>
-      <c r="H50" s="24"/>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="G50" s="24"/>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="3" t="s">
         <v>141</v>
       </c>
@@ -2325,13 +2311,12 @@
         <v>51</v>
       </c>
       <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="14">
+      <c r="E51" s="14">
         <v>11.88</v>
       </c>
-      <c r="H51" s="14"/>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="3" t="s">
         <v>142</v>
       </c>
@@ -2342,13 +2327,12 @@
         <v>52</v>
       </c>
       <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7">
+      <c r="E52" s="7">
         <v>58</v>
       </c>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="3" t="s">
         <v>143</v>
       </c>
@@ -2359,13 +2343,12 @@
         <v>53</v>
       </c>
       <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="14">
+      <c r="E53" s="14">
         <v>90</v>
       </c>
-      <c r="H53" s="14"/>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="G53" s="14"/>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="3" t="s">
         <v>144</v>
       </c>
@@ -2376,13 +2359,12 @@
         <v>54</v>
       </c>
       <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="7">
+      <c r="E54" s="7">
         <v>0</v>
       </c>
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="3" t="s">
         <v>145</v>
       </c>
@@ -2393,13 +2375,12 @@
         <v>55</v>
       </c>
       <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="14">
+      <c r="E55" s="14">
         <v>0</v>
       </c>
-      <c r="H55" s="14"/>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="G55" s="14"/>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="3" t="s">
         <v>146</v>
       </c>
@@ -2410,13 +2391,12 @@
         <v>56</v>
       </c>
       <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="7">
+      <c r="E56" s="7">
         <v>60</v>
       </c>
-      <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="3" t="s">
         <v>147</v>
       </c>
@@ -2427,13 +2407,12 @@
         <v>57</v>
       </c>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="14">
+      <c r="E57" s="14">
         <v>90</v>
       </c>
-      <c r="H57" s="14"/>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="G57" s="14"/>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="3" t="s">
         <v>148</v>
       </c>
@@ -2444,13 +2423,12 @@
         <v>58</v>
       </c>
       <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="7">
+      <c r="E58" s="7">
         <v>105</v>
       </c>
-      <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="3" t="s">
         <v>149</v>
       </c>
@@ -2461,13 +2439,12 @@
         <v>59</v>
       </c>
       <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="14">
+      <c r="E59" s="14">
         <v>60</v>
       </c>
-      <c r="H59" s="14"/>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="G59" s="14"/>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="3" t="s">
         <v>150</v>
       </c>
@@ -2478,13 +2455,12 @@
         <v>60</v>
       </c>
       <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="7">
+      <c r="E60" s="7">
         <v>225</v>
       </c>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="3" t="s">
         <v>151</v>
       </c>
@@ -2495,13 +2471,12 @@
         <v>61</v>
       </c>
       <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="7">
+      <c r="E61" s="7">
         <v>460</v>
       </c>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="3" t="s">
         <v>152</v>
       </c>
@@ -2512,13 +2487,12 @@
         <v>62</v>
       </c>
       <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="7">
+      <c r="E62" s="7">
         <v>57</v>
       </c>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="3" t="s">
         <v>153</v>
       </c>
@@ -2529,13 +2503,12 @@
         <v>63</v>
       </c>
       <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="14">
+      <c r="E63" s="14">
         <v>13.04</v>
       </c>
-      <c r="H63" s="14"/>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="3" t="s">
         <v>154</v>
       </c>
@@ -2546,13 +2519,12 @@
         <v>64</v>
       </c>
       <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="7">
+      <c r="E64" s="7">
         <v>180</v>
       </c>
-      <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="3" t="s">
         <v>155</v>
       </c>
@@ -2563,13 +2535,12 @@
         <v>65</v>
       </c>
       <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="14">
+      <c r="E65" s="14">
         <v>46</v>
       </c>
-      <c r="H65" s="14"/>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="G65" s="14"/>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="3" t="s">
         <v>156</v>
       </c>
@@ -2580,13 +2551,12 @@
         <v>66</v>
       </c>
       <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="7">
+      <c r="E66" s="7">
         <v>1150</v>
       </c>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="G66" s="7"/>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="3" t="s">
         <v>157</v>
       </c>
@@ -2597,13 +2567,12 @@
         <v>67</v>
       </c>
       <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="14">
+      <c r="E67" s="14">
         <v>8</v>
       </c>
-      <c r="H67" s="14"/>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="G67" s="14"/>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="3" t="s">
         <v>158</v>
       </c>
@@ -2614,13 +2583,12 @@
         <v>68</v>
       </c>
       <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="7">
+      <c r="E68" s="7">
         <v>0</v>
       </c>
-      <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="G68" s="7"/>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="3" t="s">
         <v>159</v>
       </c>
@@ -2631,13 +2599,12 @@
         <v>69</v>
       </c>
       <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="14">
+      <c r="E69" s="14">
         <v>775</v>
       </c>
-      <c r="H69" s="14"/>
-    </row>
-    <row r="70" spans="1:8" ht="12.6" customHeight="1">
+      <c r="G69" s="14"/>
+    </row>
+    <row r="70" spans="1:7" ht="12.6" customHeight="1">
       <c r="A70" s="3" t="s">
         <v>160</v>
       </c>
@@ -2648,13 +2615,12 @@
         <v>70</v>
       </c>
       <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="14">
+      <c r="E70" s="14">
         <v>165.54</v>
       </c>
-      <c r="H70" s="14"/>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="G70" s="14"/>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="3" t="s">
         <v>161</v>
       </c>
@@ -2665,13 +2631,12 @@
         <v>71</v>
       </c>
       <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="14">
+      <c r="E71" s="14">
         <v>470</v>
       </c>
-      <c r="H71" s="14"/>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="G71" s="14"/>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="3" t="s">
         <v>162</v>
       </c>
@@ -2682,13 +2647,12 @@
         <v>72</v>
       </c>
       <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="14">
+      <c r="E72" s="14">
         <v>117</v>
       </c>
-      <c r="H72" s="14"/>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="G72" s="14"/>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="3" t="s">
         <v>163</v>
       </c>
@@ -2699,13 +2663,12 @@
         <v>73</v>
       </c>
       <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="7">
+      <c r="E73" s="7">
         <v>50</v>
       </c>
-      <c r="H73" s="7"/>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="3" t="s">
         <v>164</v>
       </c>
@@ -2716,13 +2679,12 @@
         <v>74</v>
       </c>
       <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="14">
+      <c r="E74" s="14">
         <v>63</v>
       </c>
-      <c r="H74" s="14"/>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="G74" s="14"/>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="3" t="s">
         <v>165</v>
       </c>
@@ -2733,13 +2695,12 @@
         <v>75</v>
       </c>
       <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="14">
+      <c r="E75" s="14">
         <v>58</v>
       </c>
-      <c r="H75" s="14"/>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="G75" s="14"/>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="3" t="s">
         <v>166</v>
       </c>
@@ -2750,13 +2711,12 @@
         <v>76</v>
       </c>
       <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="14">
+      <c r="E76" s="14">
         <v>1000</v>
       </c>
-      <c r="H76" s="14"/>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="G76" s="14"/>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="3" t="s">
         <v>167</v>
       </c>
@@ -2767,13 +2727,12 @@
         <v>77</v>
       </c>
       <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="7">
+      <c r="E77" s="7">
         <v>57</v>
       </c>
-      <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="3" t="s">
         <v>168</v>
       </c>
@@ -2784,13 +2743,12 @@
         <v>78</v>
       </c>
       <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="14">
+      <c r="E78" s="14">
         <v>580</v>
       </c>
-      <c r="H78" s="14"/>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="G78" s="14"/>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="3" t="s">
         <v>169</v>
       </c>
@@ -2801,13 +2759,12 @@
         <v>79</v>
       </c>
       <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="7">
+      <c r="E79" s="7">
         <v>28</v>
       </c>
-      <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="G79" s="7"/>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="3" t="s">
         <v>170</v>
       </c>
@@ -2818,13 +2775,12 @@
         <v>80</v>
       </c>
       <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="14">
+      <c r="E80" s="14">
         <v>83</v>
       </c>
-      <c r="H80" s="14"/>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="G80" s="14"/>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="3" t="s">
         <v>171</v>
       </c>
@@ -2835,13 +2791,12 @@
         <v>81</v>
       </c>
       <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="14">
+      <c r="E81" s="14">
         <v>50</v>
       </c>
-      <c r="H81" s="14"/>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="G81" s="14"/>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="3" t="s">
         <v>172</v>
       </c>
@@ -2852,13 +2807,12 @@
         <v>82</v>
       </c>
       <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="14">
+      <c r="E82" s="14">
         <v>275</v>
       </c>
-      <c r="H82" s="14"/>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="G82" s="14"/>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="3" t="s">
         <v>173</v>
       </c>
@@ -2869,13 +2823,12 @@
         <v>83</v>
       </c>
       <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="7">
+      <c r="E83" s="7">
         <v>158</v>
       </c>
-      <c r="H83" s="7"/>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="G83" s="7"/>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="3" t="s">
         <v>174</v>
       </c>
@@ -2886,13 +2839,12 @@
         <v>84</v>
       </c>
       <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="7">
+      <c r="E84" s="7">
         <v>350</v>
       </c>
-      <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="G84" s="7"/>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="3" t="s">
         <v>175</v>
       </c>
@@ -2903,13 +2855,12 @@
         <v>85</v>
       </c>
       <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="14">
+      <c r="E85" s="14">
         <v>48</v>
       </c>
-      <c r="H85" s="14"/>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="G85" s="14"/>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="3" t="s">
         <v>176</v>
       </c>
@@ -2920,13 +2871,12 @@
         <v>86</v>
       </c>
       <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="7">
+      <c r="E86" s="7">
         <v>180</v>
       </c>
-      <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="G86" s="7"/>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="3" t="s">
         <v>177</v>
       </c>
@@ -2937,13 +2887,12 @@
         <v>282</v>
       </c>
       <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="14">
+      <c r="E87" s="14">
         <v>50</v>
       </c>
-      <c r="H87" s="14"/>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="G87" s="14"/>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="3" t="s">
         <v>178</v>
       </c>
@@ -2954,13 +2903,12 @@
         <v>87</v>
       </c>
       <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="7">
+      <c r="E88" s="7">
         <v>68.7</v>
       </c>
-      <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="G88" s="7"/>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="3" t="s">
         <v>179</v>
       </c>
@@ -2971,13 +2919,12 @@
         <v>88</v>
       </c>
       <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="14">
+      <c r="E89" s="14">
         <v>135</v>
       </c>
-      <c r="H89" s="14"/>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="G89" s="14"/>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="3" t="s">
         <v>180</v>
       </c>
@@ -2988,13 +2935,12 @@
         <v>281</v>
       </c>
       <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="14">
+      <c r="E90" s="14">
         <v>90</v>
       </c>
-      <c r="H90" s="14"/>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="G90" s="14"/>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="3" t="s">
         <v>181</v>
       </c>
@@ -3005,13 +2951,12 @@
         <v>89</v>
       </c>
       <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="7">
+      <c r="E91" s="7">
         <v>12</v>
       </c>
-      <c r="H91" s="7"/>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="G91" s="7"/>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="3" t="s">
         <v>182</v>
       </c>
@@ -3022,13 +2967,12 @@
         <v>90</v>
       </c>
       <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="14">
+      <c r="E92" s="14">
         <v>240</v>
       </c>
-      <c r="H92" s="14"/>
-    </row>
-    <row r="93" spans="1:8" ht="15" customHeight="1">
+      <c r="G92" s="14"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" customHeight="1">
       <c r="A93" s="3" t="s">
         <v>183</v>
       </c>
@@ -3039,13 +2983,12 @@
         <v>91</v>
       </c>
       <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="7">
+      <c r="E93" s="7">
         <v>220</v>
       </c>
-      <c r="H93" s="7"/>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="G93" s="7"/>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="3" t="s">
         <v>184</v>
       </c>
@@ -3056,42 +2999,38 @@
         <v>92</v>
       </c>
       <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="14">
+      <c r="E94" s="14">
         <v>140</v>
       </c>
-      <c r="H94" s="14"/>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="G94" s="14"/>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="12"/>
       <c r="B95" s="16"/>
       <c r="C95" s="10"/>
       <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="G95" s="10"/>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="F95" s="10"/>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="13"/>
       <c r="B96" s="4"/>
       <c r="C96" s="11"/>
       <c r="D96" s="13"/>
-      <c r="E96" s="13"/>
-      <c r="G96" s="11"/>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="F96" s="11"/>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="12"/>
       <c r="B97" s="16"/>
       <c r="C97" s="10"/>
       <c r="D97" s="12"/>
-      <c r="E97" s="12"/>
-      <c r="G97" s="10"/>
+      <c r="F97" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{802B1A7B-8A79-4659-8E89-ED4687920ABC}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{905F2BE5-DF0A-4B95-AB88-3FB6ABA59546}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{418FFF70-E658-4A33-B0E5-E7ED84EFB833}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{999A950D-FD0C-4F54-A4DD-65D70771F4E7}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{802B1A7B-8A79-4659-8E89-ED4687920ABC}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{905F2BE5-DF0A-4B95-AB88-3FB6ABA59546}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{418FFF70-E658-4A33-B0E5-E7ED84EFB833}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{999A950D-FD0C-4F54-A4DD-65D70771F4E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>